<commit_message>
Five range sliders added
</commit_message>
<xml_diff>
--- a/Sample Companies Financials Original Format.xlsx
+++ b/Sample Companies Financials Original Format.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="775" documentId="8_{B5691506-39FA-424E-99D4-26D7CBA25480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3C24C90A-1914-4DA1-B210-5CEABA4E03B3}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{3D767867-0467-441D-9DC3-18181976D26B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3D767867-0467-441D-9DC3-18181976D26B}"/>
   </bookViews>
   <sheets>
     <sheet name="Entered data" sheetId="1" r:id="rId1"/>
@@ -754,8 +754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2D36DD3-6B56-4F2F-A2FA-7F51CDCFAD25}">
   <dimension ref="A3:K286"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A264" workbookViewId="0">
-      <selection activeCell="A289" sqref="A289"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A264" workbookViewId="0">
+      <selection activeCell="B279" sqref="B279"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.25"/>
@@ -6409,7 +6409,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C384203C-F021-4178-95D6-38ABC9D05E39}">
   <dimension ref="A1:V61"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="11.25" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
All range sliders data sourced from database
</commit_message>
<xml_diff>
--- a/Sample Companies Financials Original Format.xlsx
+++ b/Sample Companies Financials Original Format.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d3708a04485001ab/Platform/GitHub/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="775" documentId="8_{B5691506-39FA-424E-99D4-26D7CBA25480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3C24C90A-1914-4DA1-B210-5CEABA4E03B3}"/>
+  <xr:revisionPtr revIDLastSave="776" documentId="8_{B5691506-39FA-424E-99D4-26D7CBA25480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A9E9CC46-8692-4576-900A-585D70F3CE41}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3D767867-0467-441D-9DC3-18181976D26B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{3D767867-0467-441D-9DC3-18181976D26B}"/>
   </bookViews>
   <sheets>
     <sheet name="Entered data" sheetId="1" r:id="rId1"/>
@@ -754,8 +754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2D36DD3-6B56-4F2F-A2FA-7F51CDCFAD25}">
   <dimension ref="A3:K286"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A264" workbookViewId="0">
-      <selection activeCell="B279" sqref="B279"/>
+    <sheetView showGridLines="0" topLeftCell="A264" workbookViewId="0">
+      <selection activeCell="H276" sqref="H276"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.25"/>
@@ -6407,9 +6407,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C384203C-F021-4178-95D6-38ABC9D05E39}">
-  <dimension ref="A1:V61"/>
+  <dimension ref="A1:V63"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G38" workbookViewId="0">
+      <selection activeCell="P63" sqref="P63"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="11.25" x14ac:dyDescent="0.25"/>
   <cols>
@@ -10256,6 +10258,12 @@
         <v>0.43897108271687962</v>
       </c>
     </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="P63" s="12">
+        <f>MAX(P2:P61)</f>
+        <v>2.4563106796116503</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added tile filtering functionality using range sliders and applied to four companies
</commit_message>
<xml_diff>
--- a/Sample Companies Financials Original Format.xlsx
+++ b/Sample Companies Financials Original Format.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d3708a04485001ab/Platform/GitHub/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="816" documentId="8_{B5691506-39FA-424E-99D4-26D7CBA25480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{578CF9E8-7396-4765-A0AB-58BEF92A7147}"/>
+  <xr:revisionPtr revIDLastSave="1005" documentId="8_{B5691506-39FA-424E-99D4-26D7CBA25480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7A37C57A-99F1-47E5-A458-96A8A07A4D51}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{3D767867-0467-441D-9DC3-18181976D26B}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="84">
   <si>
     <t>Turnover</t>
   </si>
@@ -272,14 +272,36 @@
   <si>
     <t>Solvency_Ratio</t>
   </si>
+  <si>
+    <t>Profits</t>
+  </si>
+  <si>
+    <t>Assets</t>
+  </si>
+  <si>
+    <t>Cashflow</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Aston Martin</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="166" formatCode="0.000%"/>
+    <numFmt numFmtId="167" formatCode="0.0000%"/>
+    <numFmt numFmtId="177" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="188" formatCode="#,##0.000000000000000"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -339,12 +361,24 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -360,7 +394,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -420,6 +454,54 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="188" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -6410,15 +6492,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C384203C-F021-4178-95D6-38ABC9D05E39}">
-  <dimension ref="A1:V64"/>
+  <dimension ref="A1:V73"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="K79" sqref="K79"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="11.25" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.7109375" style="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" style="15"/>
-    <col min="3" max="12" width="12.7109375" style="2"/>
+    <col min="3" max="6" width="12.7109375" style="2"/>
+    <col min="7" max="7" width="15.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="2"/>
+    <col min="9" max="9" width="15.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="12.7109375" style="2"/>
     <col min="13" max="15" width="12.7109375" style="12"/>
     <col min="16" max="16" width="12.7109375" style="20"/>
     <col min="17" max="20" width="12.7109375" style="12"/>
@@ -6487,68 +6575,68 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+    <row r="2" spans="1:22" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="15">
+      <c r="B2" s="21">
         <v>2023</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="22">
         <v>1633000</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="22">
         <v>3173000</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="22">
         <v>2616000</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="22">
         <v>-88000</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="22">
         <v>-228000</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2" s="22">
         <v>-54500</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2" s="22">
         <v>902000</v>
       </c>
-      <c r="J2" s="2">
+      <c r="J2" s="22">
         <v>155000</v>
       </c>
-      <c r="K2" s="2">
+      <c r="K2" s="22">
         <v>1069000</v>
       </c>
-      <c r="L2" s="2">
+      <c r="L2" s="22">
         <v>923000</v>
       </c>
-      <c r="M2" s="12">
+      <c r="M2" s="23">
         <v>-5.3888548683404779E-2</v>
       </c>
-      <c r="N2" s="12">
+      <c r="N2" s="23">
         <v>-0.13962033067973056</v>
       </c>
-      <c r="O2" s="12">
+      <c r="O2" s="23">
         <v>-3.3374157991426824E-2</v>
       </c>
-      <c r="P2" s="20">
+      <c r="P2" s="24">
         <v>-0.56774193548387097</v>
       </c>
-      <c r="Q2" s="12">
+      <c r="Q2" s="23">
         <v>-7.1856287425149698E-2</v>
       </c>
-      <c r="R2" s="12">
+      <c r="R2" s="23">
         <v>0.28427355814686417</v>
       </c>
-      <c r="S2" s="12">
+      <c r="S2" s="23">
         <v>1.1581798483206933</v>
       </c>
-      <c r="T2" s="12">
+      <c r="T2" s="23">
         <v>0.28427355814686417</v>
       </c>
-      <c r="V2" s="15" t="s">
+      <c r="V2" s="21" t="s">
         <v>53</v>
       </c>
     </row>
@@ -6812,69 +6900,69 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+    <row r="7" spans="1:22" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="21">
         <v>2023</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="22">
         <v>1749000</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="22">
         <v>1898000</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="22">
         <v>1506000</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="22">
         <v>120000</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="22">
         <v>124000</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="22">
         <v>148000</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="22">
         <v>392000</v>
       </c>
-      <c r="J7" s="2">
+      <c r="J7" s="22">
         <v>24000</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K7" s="22">
         <v>611000</v>
       </c>
-      <c r="L7" s="2">
+      <c r="L7" s="22">
         <v>392000</v>
       </c>
-      <c r="M7" s="12">
+      <c r="M7" s="23">
         <v>6.86106346483705E-2</v>
       </c>
-      <c r="N7" s="12">
+      <c r="N7" s="23">
         <v>7.0897655803316181E-2</v>
       </c>
-      <c r="O7" s="12">
+      <c r="O7" s="23">
         <v>8.4619782732990284E-2</v>
       </c>
-      <c r="P7" s="20">
+      <c r="P7" s="24">
         <v>5</v>
       </c>
-      <c r="Q7" s="12">
+      <c r="Q7" s="23">
         <v>6.5331928345626969E-2</v>
       </c>
-      <c r="R7" s="12">
+      <c r="R7" s="23">
         <v>0.2065331928345627</v>
       </c>
-      <c r="S7" s="12">
+      <c r="S7" s="23">
         <v>1.5586734693877551</v>
       </c>
-      <c r="T7" s="12">
+      <c r="T7" s="23">
         <v>0.2065331928345627</v>
       </c>
-      <c r="U7" s="18"/>
-      <c r="V7" s="15" t="s">
+      <c r="U7" s="25"/>
+      <c r="V7" s="21" t="s">
         <v>66</v>
       </c>
     </row>
@@ -7142,69 +7230,69 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
+    <row r="12" spans="1:22" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="15">
+      <c r="B12" s="21">
         <v>2023</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="22">
         <v>420000</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="22">
         <v>8290000</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="22">
         <v>2765000</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="22">
         <v>323000</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12" s="22">
         <v>-1038000</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12" s="22">
         <v>240000</v>
       </c>
-      <c r="I12" s="2">
+      <c r="I12" s="22">
         <v>5512000</v>
       </c>
-      <c r="J12" s="2">
+      <c r="J12" s="22">
         <v>90000</v>
       </c>
-      <c r="K12" s="2">
+      <c r="K12" s="22">
         <v>1985000</v>
       </c>
-      <c r="L12" s="2">
+      <c r="L12" s="22">
         <v>5525000</v>
       </c>
-      <c r="M12" s="12">
+      <c r="M12" s="23">
         <v>0.76904761904761909</v>
       </c>
-      <c r="N12" s="12">
+      <c r="N12" s="23">
         <v>-2.4714285714285715</v>
       </c>
-      <c r="O12" s="12">
+      <c r="O12" s="23">
         <v>0.5714285714285714</v>
       </c>
-      <c r="P12" s="20">
+      <c r="P12" s="24">
         <v>3.588888888888889</v>
       </c>
-      <c r="Q12" s="12">
+      <c r="Q12" s="23">
         <v>-0.12521109770808203</v>
       </c>
-      <c r="R12" s="12">
+      <c r="R12" s="23">
         <v>0.66489746682750306</v>
       </c>
-      <c r="S12" s="12">
+      <c r="S12" s="23">
         <v>0.35927601809954751</v>
       </c>
-      <c r="T12" s="12">
+      <c r="T12" s="23">
         <v>0.66489746682750306</v>
       </c>
-      <c r="U12" s="18"/>
-      <c r="V12" s="15" t="s">
+      <c r="U12" s="25"/>
+      <c r="V12" s="21" t="s">
         <v>71</v>
       </c>
     </row>
@@ -7472,69 +7560,69 @@
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A17" s="15" t="s">
+    <row r="17" spans="1:22" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="15">
+      <c r="B17" s="21">
         <v>2023</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="22">
         <v>218234</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="22">
         <v>234837</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="22">
         <v>68800</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17" s="22">
         <v>86204</v>
       </c>
-      <c r="G17" s="2">
+      <c r="G17" s="22">
         <v>68219</v>
       </c>
-      <c r="H17" s="2">
+      <c r="H17" s="22">
         <v>102229</v>
       </c>
-      <c r="I17" s="2">
+      <c r="I17" s="22">
         <v>166037</v>
       </c>
-      <c r="J17" s="2">
+      <c r="J17" s="22">
         <v>952</v>
       </c>
-      <c r="K17" s="2">
+      <c r="K17" s="22">
         <v>10866</v>
       </c>
-      <c r="L17" s="2">
+      <c r="L17" s="22">
         <v>166037</v>
       </c>
-      <c r="M17" s="12">
+      <c r="M17" s="23">
         <v>0.39500719411274138</v>
       </c>
-      <c r="N17" s="12">
+      <c r="N17" s="23">
         <v>0.31259565420603574</v>
       </c>
-      <c r="O17" s="12">
+      <c r="O17" s="23">
         <v>0.46843754868627252</v>
       </c>
-      <c r="P17" s="20">
+      <c r="P17" s="24">
         <v>90.550420168067234</v>
       </c>
-      <c r="Q17" s="12">
+      <c r="Q17" s="23">
         <v>0.29049510937373585</v>
       </c>
-      <c r="R17" s="12">
+      <c r="R17" s="23">
         <v>0.70703083415305079</v>
       </c>
-      <c r="S17" s="12">
+      <c r="S17" s="23">
         <v>6.5443244578015744E-2</v>
       </c>
-      <c r="T17" s="12">
+      <c r="T17" s="23">
         <v>0.70703083415305079</v>
       </c>
-      <c r="U17" s="18"/>
-      <c r="V17" s="15" t="s">
+      <c r="U17" s="25"/>
+      <c r="V17" s="21" t="s">
         <v>75</v>
       </c>
     </row>
@@ -7802,68 +7890,68 @@
         <v>77</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A22" s="15" t="s">
+    <row r="22" spans="1:22" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="15">
+      <c r="B22" s="21">
         <v>2023</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="22">
         <v>679800</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22" s="22">
         <v>512500</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22" s="22">
         <v>646500</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F22" s="22">
         <v>111900</v>
       </c>
-      <c r="G22" s="2">
+      <c r="G22" s="22">
         <v>115000</v>
       </c>
-      <c r="H22" s="2">
+      <c r="H22" s="22">
         <v>90600</v>
       </c>
-      <c r="I22" s="2">
+      <c r="I22" s="22">
         <v>-134000</v>
       </c>
-      <c r="J22" s="2">
+      <c r="J22" s="22">
         <v>28200</v>
       </c>
-      <c r="K22" s="2">
+      <c r="K22" s="22">
         <v>494100</v>
       </c>
-      <c r="L22" s="2">
+      <c r="L22" s="22">
         <v>-134000</v>
       </c>
-      <c r="M22" s="12">
+      <c r="M22" s="23">
         <v>0.16460723742277139</v>
       </c>
-      <c r="N22" s="12">
+      <c r="N22" s="23">
         <v>0.1691674021771109</v>
       </c>
-      <c r="O22" s="12">
+      <c r="O22" s="23">
         <v>0.13327449249779347</v>
       </c>
-      <c r="P22" s="20">
+      <c r="P22" s="24">
         <v>3.9680851063829787</v>
       </c>
-      <c r="Q22" s="12">
+      <c r="Q22" s="23">
         <v>0.22439024390243903</v>
       </c>
-      <c r="R22" s="12">
+      <c r="R22" s="23">
         <v>-0.26146341463414635</v>
       </c>
-      <c r="S22" s="12">
+      <c r="S22" s="23">
         <v>-3.687313432835821</v>
       </c>
-      <c r="T22" s="12">
+      <c r="T22" s="23">
         <v>-0.26146341463414635</v>
       </c>
-      <c r="U22" s="18"/>
+      <c r="U22" s="25"/>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
@@ -8429,68 +8517,68 @@
       </c>
       <c r="U31" s="18"/>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A32" s="15" t="s">
+    <row r="32" spans="1:22" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="B32" s="15">
+      <c r="B32" s="21">
         <v>2023</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C32" s="22">
         <v>1000000</v>
       </c>
-      <c r="D32" s="2">
+      <c r="D32" s="22">
         <v>992600</v>
       </c>
-      <c r="E32" s="2">
+      <c r="E32" s="22">
         <v>588400</v>
       </c>
-      <c r="F32" s="2">
+      <c r="F32" s="22">
         <v>191000</v>
       </c>
-      <c r="G32" s="2">
+      <c r="G32" s="22">
         <v>129000</v>
       </c>
-      <c r="H32" s="2">
+      <c r="H32" s="22">
         <v>32100</v>
       </c>
-      <c r="I32" s="2">
+      <c r="I32" s="22">
         <v>404200</v>
       </c>
-      <c r="J32" s="2">
+      <c r="J32" s="22">
         <v>19000</v>
       </c>
-      <c r="K32" s="2">
+      <c r="K32" s="22">
         <v>417700</v>
       </c>
-      <c r="L32" s="2">
+      <c r="L32" s="22">
         <v>404200</v>
       </c>
-      <c r="M32" s="12">
+      <c r="M32" s="23">
         <v>0.191</v>
       </c>
-      <c r="N32" s="12">
+      <c r="N32" s="23">
         <v>0.129</v>
       </c>
-      <c r="O32" s="12">
+      <c r="O32" s="23">
         <v>3.2099999999999997E-2</v>
       </c>
-      <c r="P32" s="20">
+      <c r="P32" s="24">
         <v>10.052631578947368</v>
       </c>
-      <c r="Q32" s="12">
+      <c r="Q32" s="23">
         <v>0.12996171670360668</v>
       </c>
-      <c r="R32" s="12">
+      <c r="R32" s="23">
         <v>0.40721337900463428</v>
       </c>
-      <c r="S32" s="12">
+      <c r="S32" s="23">
         <v>1.0333993072736269</v>
       </c>
-      <c r="T32" s="12">
+      <c r="T32" s="23">
         <v>0.40721337900463428</v>
       </c>
-      <c r="U32" s="18"/>
+      <c r="U32" s="25"/>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" s="15" t="s">
@@ -8744,68 +8832,68 @@
       </c>
       <c r="U36" s="18"/>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A37" s="15" t="s">
+    <row r="37" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="B37" s="15">
+      <c r="B37" s="21">
         <v>2023</v>
       </c>
-      <c r="C37" s="2">
+      <c r="C37" s="22">
         <v>470800</v>
       </c>
-      <c r="D37" s="2">
+      <c r="D37" s="22">
         <v>326800</v>
       </c>
-      <c r="E37" s="2">
+      <c r="E37" s="22">
         <v>91700</v>
       </c>
-      <c r="F37" s="2">
+      <c r="F37" s="22">
         <v>175300</v>
       </c>
-      <c r="G37" s="2">
+      <c r="G37" s="22">
         <v>134700</v>
       </c>
-      <c r="H37" s="2">
+      <c r="H37" s="22">
         <v>179100</v>
       </c>
-      <c r="I37" s="2">
+      <c r="I37" s="22">
         <v>235100</v>
       </c>
-      <c r="J37" s="2">
+      <c r="J37" s="22">
         <v>900</v>
       </c>
-      <c r="K37" s="2">
+      <c r="K37" s="22">
         <v>40000</v>
       </c>
-      <c r="L37" s="2">
+      <c r="L37" s="22">
         <v>235100</v>
       </c>
-      <c r="M37" s="12">
+      <c r="M37" s="23">
         <v>0.37234494477485131</v>
       </c>
-      <c r="N37" s="12">
+      <c r="N37" s="23">
         <v>0.2861087510620221</v>
       </c>
-      <c r="O37" s="12">
+      <c r="O37" s="23">
         <v>0.38041631265930331</v>
       </c>
-      <c r="P37" s="20">
+      <c r="P37" s="24">
         <v>194.77777777777777</v>
       </c>
-      <c r="Q37" s="12">
+      <c r="Q37" s="23">
         <v>0.41217870257037942</v>
       </c>
-      <c r="R37" s="12">
+      <c r="R37" s="23">
         <v>0.71940024479804165</v>
       </c>
-      <c r="S37" s="12">
+      <c r="S37" s="23">
         <v>0.17014036580178649</v>
       </c>
-      <c r="T37" s="12">
+      <c r="T37" s="23">
         <v>0.71940024479804165</v>
       </c>
-      <c r="U37" s="18"/>
+      <c r="U37" s="25"/>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" s="15" t="s">
@@ -9059,68 +9147,68 @@
       </c>
       <c r="U41" s="18"/>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A42" s="15" t="s">
+    <row r="42" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="B42" s="15">
+      <c r="B42" s="21">
         <v>2023</v>
       </c>
-      <c r="C42" s="2">
+      <c r="C42" s="22">
         <v>7583000</v>
       </c>
-      <c r="D42" s="2">
+      <c r="D42" s="22">
         <v>1904000</v>
       </c>
-      <c r="E42" s="2">
+      <c r="E42" s="22">
         <v>1234000</v>
       </c>
-      <c r="F42" s="2">
+      <c r="F42" s="22">
         <v>197000</v>
       </c>
-      <c r="G42" s="2">
+      <c r="G42" s="22">
         <v>138000</v>
       </c>
-      <c r="H42" s="2">
+      <c r="H42" s="22">
         <v>151700</v>
       </c>
-      <c r="I42" s="2">
+      <c r="I42" s="22">
         <v>670000</v>
       </c>
-      <c r="J42" s="2">
+      <c r="J42" s="22">
         <v>8000</v>
       </c>
-      <c r="K42" s="2">
+      <c r="K42" s="22">
         <v>159000</v>
       </c>
-      <c r="L42" s="2">
+      <c r="L42" s="22">
         <v>670000</v>
       </c>
-      <c r="M42" s="12">
+      <c r="M42" s="23">
         <v>2.5979163919293155E-2</v>
       </c>
-      <c r="N42" s="12">
+      <c r="N42" s="23">
         <v>1.8198602136357642E-2</v>
       </c>
-      <c r="O42" s="12">
+      <c r="O42" s="23">
         <v>2.0005274957140974E-2</v>
       </c>
-      <c r="P42" s="20">
+      <c r="P42" s="24">
         <v>24.625</v>
       </c>
-      <c r="Q42" s="12">
+      <c r="Q42" s="23">
         <v>7.2478991596638662E-2</v>
       </c>
-      <c r="R42" s="12">
+      <c r="R42" s="23">
         <v>0.35189075630252103</v>
       </c>
-      <c r="S42" s="12">
+      <c r="S42" s="23">
         <v>0.2373134328358209</v>
       </c>
-      <c r="T42" s="12">
+      <c r="T42" s="23">
         <v>0.35189075630252103</v>
       </c>
-      <c r="U42" s="18"/>
+      <c r="U42" s="25"/>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" s="15" t="s">
@@ -9374,68 +9462,68 @@
       </c>
       <c r="U46" s="18"/>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A47" s="15" t="s">
+    <row r="47" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="B47" s="15">
+      <c r="B47" s="21">
         <v>2023</v>
       </c>
-      <c r="C47" s="2">
+      <c r="C47" s="22">
         <v>405839</v>
       </c>
-      <c r="D47" s="2">
+      <c r="D47" s="22">
         <v>754231</v>
       </c>
-      <c r="E47" s="2">
+      <c r="E47" s="22">
         <v>354364</v>
       </c>
-      <c r="F47" s="2">
+      <c r="F47" s="22">
         <v>60828</v>
       </c>
-      <c r="G47" s="2">
+      <c r="G47" s="22">
         <v>21060</v>
       </c>
-      <c r="H47" s="2">
+      <c r="H47" s="22">
         <v>-7145</v>
       </c>
-      <c r="I47" s="2">
+      <c r="I47" s="22">
         <v>399867</v>
       </c>
-      <c r="J47" s="2">
+      <c r="J47" s="22">
         <v>5462</v>
       </c>
-      <c r="K47" s="2">
+      <c r="K47" s="22">
         <v>133533</v>
       </c>
-      <c r="L47" s="2">
+      <c r="L47" s="22">
         <v>399867</v>
       </c>
-      <c r="M47" s="12">
+      <c r="M47" s="23">
         <v>0.14988209610214889</v>
       </c>
-      <c r="N47" s="12">
+      <c r="N47" s="23">
         <v>5.1892499242310375E-2</v>
       </c>
-      <c r="O47" s="12">
+      <c r="O47" s="23">
         <v>-1.7605503660318499E-2</v>
       </c>
-      <c r="P47" s="20">
+      <c r="P47" s="24">
         <v>11.136580007323325</v>
       </c>
-      <c r="Q47" s="12">
+      <c r="Q47" s="23">
         <v>2.7922479982923003E-2</v>
       </c>
-      <c r="R47" s="12">
+      <c r="R47" s="23">
         <v>0.53016516160168436</v>
       </c>
-      <c r="S47" s="12">
+      <c r="S47" s="23">
         <v>0.33394353622579509</v>
       </c>
-      <c r="T47" s="12">
+      <c r="T47" s="23">
         <v>0.53016516160168436</v>
       </c>
-      <c r="U47" s="18"/>
+      <c r="U47" s="25"/>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48" s="15" t="s">
@@ -9689,68 +9777,68 @@
       </c>
       <c r="U51" s="18"/>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A52" s="15" t="s">
+    <row r="52" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="B52" s="15">
+      <c r="B52" s="21">
         <v>2023</v>
       </c>
-      <c r="C52" s="2">
+      <c r="C52" s="22">
         <v>3624000</v>
       </c>
-      <c r="D52" s="2">
+      <c r="D52" s="22">
         <v>4191000</v>
       </c>
-      <c r="E52" s="2">
+      <c r="E52" s="22">
         <v>2363000</v>
       </c>
-      <c r="F52" s="2">
+      <c r="F52" s="22">
         <v>321000</v>
       </c>
-      <c r="G52" s="2">
+      <c r="G52" s="22">
         <v>210000</v>
       </c>
-      <c r="H52" s="2">
+      <c r="H52" s="22">
         <v>1786000</v>
       </c>
-      <c r="I52" s="2">
+      <c r="I52" s="22">
         <v>354000</v>
       </c>
-      <c r="J52" s="2">
+      <c r="J52" s="22">
         <v>62000</v>
       </c>
-      <c r="K52" s="2">
+      <c r="K52" s="22">
         <v>855000</v>
       </c>
-      <c r="L52" s="2">
+      <c r="L52" s="22">
         <v>1828000</v>
       </c>
-      <c r="M52" s="12">
+      <c r="M52" s="23">
         <v>8.8576158940397345E-2</v>
       </c>
-      <c r="N52" s="12">
+      <c r="N52" s="23">
         <v>5.7947019867549666E-2</v>
       </c>
-      <c r="O52" s="12">
+      <c r="O52" s="23">
         <v>0.49282560706401768</v>
       </c>
-      <c r="P52" s="20">
+      <c r="P52" s="24">
         <v>5.17741935483871</v>
       </c>
-      <c r="Q52" s="12">
+      <c r="Q52" s="23">
         <v>5.0107372942018613E-2</v>
       </c>
-      <c r="R52" s="12">
+      <c r="R52" s="23">
         <v>8.4466714387974234E-2</v>
       </c>
-      <c r="S52" s="12">
+      <c r="S52" s="23">
         <v>0.46772428884026257</v>
       </c>
-      <c r="T52" s="12">
+      <c r="T52" s="23">
         <v>8.4466714387974234E-2</v>
       </c>
-      <c r="U52" s="18"/>
+      <c r="U52" s="25"/>
     </row>
     <row r="53" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A53" s="15" t="s">
@@ -10004,68 +10092,68 @@
       </c>
       <c r="U56" s="18"/>
     </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A57" s="15" t="s">
+    <row r="57" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="B57" s="15">
+      <c r="B57" s="21">
         <v>2023</v>
       </c>
-      <c r="C57" s="2">
+      <c r="C57" s="22">
         <v>14933000</v>
       </c>
-      <c r="D57" s="2">
+      <c r="D57" s="22">
         <v>7029000</v>
       </c>
-      <c r="E57" s="2">
+      <c r="E57" s="22">
         <v>4490000</v>
       </c>
-      <c r="F57" s="2">
+      <c r="F57" s="22">
         <v>505000</v>
       </c>
-      <c r="G57" s="2">
+      <c r="G57" s="22">
         <v>264000</v>
       </c>
-      <c r="H57" s="2">
+      <c r="H57" s="22">
         <v>-28000</v>
       </c>
-      <c r="I57" s="2">
+      <c r="I57" s="22">
         <v>2539000</v>
       </c>
-      <c r="J57" s="2">
+      <c r="J57" s="22">
         <v>90000</v>
       </c>
-      <c r="K57" s="2">
+      <c r="K57" s="22">
         <v>1491000</v>
       </c>
-      <c r="L57" s="2">
+      <c r="L57" s="22">
         <v>2539000</v>
       </c>
-      <c r="M57" s="12">
+      <c r="M57" s="23">
         <v>3.3817719145516643E-2</v>
       </c>
-      <c r="N57" s="12">
+      <c r="N57" s="23">
         <v>1.7678966048349294E-2</v>
       </c>
-      <c r="O57" s="12">
+      <c r="O57" s="23">
         <v>-1.875041853612804E-3</v>
       </c>
-      <c r="P57" s="20">
+      <c r="P57" s="24">
         <v>5.6111111111111107</v>
       </c>
-      <c r="Q57" s="12">
+      <c r="Q57" s="23">
         <v>3.7558685446009391E-2</v>
       </c>
-      <c r="R57" s="12">
+      <c r="R57" s="23">
         <v>0.36121781192203728</v>
       </c>
-      <c r="S57" s="12">
+      <c r="S57" s="23">
         <v>0.58723907050019697</v>
       </c>
-      <c r="T57" s="12">
+      <c r="T57" s="23">
         <v>0.36121781192203728</v>
       </c>
-      <c r="U57" s="18"/>
+      <c r="U57" s="25"/>
     </row>
     <row r="58" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A58" s="15" t="s">
@@ -10335,6 +10423,146 @@
         <v>14933000</v>
       </c>
     </row>
+    <row r="66" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="F66" s="12"/>
+      <c r="H66" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="I66" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="J66" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K66" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="67" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E67" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F67" s="12"/>
+      <c r="H67" s="2">
+        <v>218234</v>
+      </c>
+      <c r="I67" s="2">
+        <v>1633000</v>
+      </c>
+      <c r="J67" s="2">
+        <v>420000</v>
+      </c>
+      <c r="K67" s="2">
+        <v>14933000</v>
+      </c>
+      <c r="L67" s="2" t="b">
+        <f t="shared" ref="L67:L69" si="0">K67&gt;J67</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E68" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F68" s="12"/>
+      <c r="H68" s="2">
+        <v>234837</v>
+      </c>
+      <c r="I68" s="2">
+        <v>3173000</v>
+      </c>
+      <c r="J68" s="2">
+        <v>8290000</v>
+      </c>
+      <c r="K68" s="2">
+        <v>8290000</v>
+      </c>
+      <c r="L68" s="2" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E69" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G69" s="29"/>
+      <c r="H69" s="31">
+        <v>-5.38885486834047</v>
+      </c>
+      <c r="I69" s="26">
+        <v>-5.3888548683404702E-2</v>
+      </c>
+      <c r="J69" s="35">
+        <v>0.76904761904761909</v>
+      </c>
+      <c r="K69" s="36">
+        <v>76905</v>
+      </c>
+      <c r="L69" s="2" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E70" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G70" s="30"/>
+      <c r="H70" s="31">
+        <v>-3.3374157991426801</v>
+      </c>
+      <c r="I70" s="28">
+        <v>-3.3374157991426803E-2</v>
+      </c>
+      <c r="J70" s="34">
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="K70" s="33">
+        <v>57143</v>
+      </c>
+      <c r="L70" s="2" t="b">
+        <f>K70&gt;J70</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E71" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G71" s="32">
+        <f>H71/100</f>
+        <v>-0.56774193548386997</v>
+      </c>
+      <c r="H71" s="27">
+        <v>-56.774193548386997</v>
+      </c>
+      <c r="I71" s="32">
+        <v>-0.56774193548387097</v>
+      </c>
+      <c r="J71" s="9">
+        <v>3.588888888888889</v>
+      </c>
+      <c r="K71" s="2">
+        <v>19478</v>
+      </c>
+      <c r="L71" s="2" t="b">
+        <f>K71&gt;J71</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="G72" s="2" t="b">
+        <f>G71&lt;I71</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="G73" s="2" t="b">
+        <f>I71&lt;G71</f>
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>